<commit_message>
Got correct sample sheet spreadsheet from Claire.  Reran code to get corrected sampling information CSV file.  Finished code for reading and organizing family taxonomy data, and created a CSV file with this info.
</commit_message>
<xml_diff>
--- a/RiceRivers/bacteria/orig_data_files/2019_RiceRiversCenter_SampleSheet.xlsx
+++ b/RiceRivers/bacteria/orig_data_files/2019_RiceRiversCenter_SampleSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/LaCie/2019 Dissertation Data/2019_08_21_RiceRIversDissertation/2019_RiceRivers_ModelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BDD88BD-0CDB-8447-A92B-C3B0720E452C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F132D504-C2E2-564F-8782-BFC5530099DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="3020" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12880" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="324">
   <si>
     <t>Location</t>
   </si>
@@ -742,9 +742,6 @@
     <t>RRR5C19CS</t>
   </si>
   <si>
-    <t>RRWC19CS</t>
-  </si>
-  <si>
     <t>RRWC19CSrep2</t>
   </si>
   <si>
@@ -965,6 +962,39 @@
   </si>
   <si>
     <t>ActualCollectedADD</t>
+  </si>
+  <si>
+    <t>RRS1C20CS</t>
+  </si>
+  <si>
+    <t>RRS2C20CS</t>
+  </si>
+  <si>
+    <t>RRS3C20CS</t>
+  </si>
+  <si>
+    <t>RRS4C20CS</t>
+  </si>
+  <si>
+    <t>RRS5C20CS</t>
+  </si>
+  <si>
+    <t>RRR1C20CS</t>
+  </si>
+  <si>
+    <t>RRR2C20CS</t>
+  </si>
+  <si>
+    <t>RRWC20CS</t>
+  </si>
+  <si>
+    <t>RRMC20CS</t>
+  </si>
+  <si>
+    <t>RRMC21CS</t>
+  </si>
+  <si>
+    <t>RRWC19CS1</t>
   </si>
 </sst>
 </file>
@@ -1457,8 +1487,8 @@
   <dimension ref="A1:K834"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H237" sqref="H237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1476,7 +1506,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>3</v>
@@ -1485,16 +1515,16 @@
         <v>0</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F1" s="24" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>296</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16">
@@ -1505,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>28</v>
@@ -1520,7 +1550,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16">
@@ -1531,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>28</v>
@@ -1546,7 +1576,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16">
@@ -1557,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>28</v>
@@ -1572,7 +1602,7 @@
         <v>6</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16">
@@ -1583,7 +1613,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>28</v>
@@ -1598,7 +1628,7 @@
         <v>6</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16">
@@ -1609,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>28</v>
@@ -1624,7 +1654,7 @@
         <v>6</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16">
@@ -1635,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>28</v>
@@ -1650,7 +1680,7 @@
         <v>6</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16">
@@ -1661,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>28</v>
@@ -1676,7 +1706,7 @@
         <v>6</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16">
@@ -1687,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>28</v>
@@ -1702,7 +1732,7 @@
         <v>6</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16">
@@ -1713,7 +1743,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>28</v>
@@ -1728,7 +1758,7 @@
         <v>6</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16">
@@ -1739,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>28</v>
@@ -1754,7 +1784,7 @@
         <v>6</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16">
@@ -1765,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>28</v>
@@ -1791,7 +1821,7 @@
         <v>268</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>28</v>
@@ -1817,7 +1847,7 @@
         <v>268</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>28</v>
@@ -1843,7 +1873,7 @@
         <v>268</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>28</v>
@@ -1869,7 +1899,7 @@
         <v>268</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>28</v>
@@ -1895,7 +1925,7 @@
         <v>268</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>28</v>
@@ -1921,7 +1951,7 @@
         <v>268</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>28</v>
@@ -1947,7 +1977,7 @@
         <v>268</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>28</v>
@@ -1973,7 +2003,7 @@
         <v>268</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>28</v>
@@ -1999,7 +2029,7 @@
         <v>268</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>28</v>
@@ -2025,7 +2055,7 @@
         <v>268</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>28</v>
@@ -2051,7 +2081,7 @@
         <v>268</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>28</v>
@@ -2077,7 +2107,7 @@
         <v>268</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>28</v>
@@ -2103,7 +2133,7 @@
         <v>516</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>28</v>
@@ -2129,7 +2159,7 @@
         <v>516</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>28</v>
@@ -2155,7 +2185,7 @@
         <v>516</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>28</v>
@@ -2181,7 +2211,7 @@
         <v>516</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>28</v>
@@ -2207,7 +2237,7 @@
         <v>516</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>28</v>
@@ -2233,7 +2263,7 @@
         <v>516</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>28</v>
@@ -2259,7 +2289,7 @@
         <v>516</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>28</v>
@@ -2285,7 +2315,7 @@
         <v>516</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>28</v>
@@ -2311,7 +2341,7 @@
         <v>516</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>28</v>
@@ -2337,7 +2367,7 @@
         <v>516</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>28</v>
@@ -2363,7 +2393,7 @@
         <v>516</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>28</v>
@@ -2389,7 +2419,7 @@
         <v>516</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>28</v>
@@ -2415,7 +2445,7 @@
         <v>741</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>28</v>
@@ -2441,7 +2471,7 @@
         <v>741</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>28</v>
@@ -2467,7 +2497,7 @@
         <v>741</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>28</v>
@@ -2493,7 +2523,7 @@
         <v>741</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>28</v>
@@ -2519,7 +2549,7 @@
         <v>741</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>28</v>
@@ -2545,7 +2575,7 @@
         <v>741</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>28</v>
@@ -2571,7 +2601,7 @@
         <v>741</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>28</v>
@@ -2597,7 +2627,7 @@
         <v>741</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>28</v>
@@ -2623,7 +2653,7 @@
         <v>741</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>28</v>
@@ -2649,7 +2679,7 @@
         <v>741</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>28</v>
@@ -2675,7 +2705,7 @@
         <v>741</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>28</v>
@@ -2701,7 +2731,7 @@
         <v>741</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>28</v>
@@ -2727,7 +2757,7 @@
         <v>1012</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>28</v>
@@ -2753,7 +2783,7 @@
         <v>1012</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>28</v>
@@ -2779,7 +2809,7 @@
         <v>1012</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>28</v>
@@ -2805,7 +2835,7 @@
         <v>1012</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>28</v>
@@ -2831,7 +2861,7 @@
         <v>1012</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>28</v>
@@ -2857,7 +2887,7 @@
         <v>1012</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>28</v>
@@ -2883,7 +2913,7 @@
         <v>1012</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>28</v>
@@ -2909,7 +2939,7 @@
         <v>1012</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>28</v>
@@ -2935,7 +2965,7 @@
         <v>1012</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>28</v>
@@ -2961,7 +2991,7 @@
         <v>1012</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>28</v>
@@ -2987,7 +3017,7 @@
         <v>1012</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>28</v>
@@ -3013,7 +3043,7 @@
         <v>1012</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>28</v>
@@ -3039,7 +3069,7 @@
         <v>1278</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>28</v>
@@ -3065,7 +3095,7 @@
         <v>1278</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>28</v>
@@ -3091,7 +3121,7 @@
         <v>1278</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>28</v>
@@ -3117,7 +3147,7 @@
         <v>1278</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>28</v>
@@ -3143,7 +3173,7 @@
         <v>1278</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>28</v>
@@ -3169,7 +3199,7 @@
         <v>1278</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>28</v>
@@ -3195,7 +3225,7 @@
         <v>1278</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>28</v>
@@ -3221,7 +3251,7 @@
         <v>1278</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>28</v>
@@ -3247,7 +3277,7 @@
         <v>1513</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>28</v>
@@ -3273,7 +3303,7 @@
         <v>1513</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>28</v>
@@ -3299,7 +3329,7 @@
         <v>1513</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>28</v>
@@ -3325,7 +3355,7 @@
         <v>1513</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>28</v>
@@ -3351,7 +3381,7 @@
         <v>1513</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>28</v>
@@ -3377,7 +3407,7 @@
         <v>1513</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>28</v>
@@ -3403,7 +3433,7 @@
         <v>1513</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>28</v>
@@ -3429,7 +3459,7 @@
         <v>1513</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>28</v>
@@ -3455,7 +3485,7 @@
         <v>1827</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>28</v>
@@ -3481,7 +3511,7 @@
         <v>1827</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>28</v>
@@ -3507,7 +3537,7 @@
         <v>1827</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>28</v>
@@ -3533,7 +3563,7 @@
         <v>1827</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>28</v>
@@ -3559,7 +3589,7 @@
         <v>1827</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>28</v>
@@ -3585,7 +3615,7 @@
         <v>1827</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>28</v>
@@ -3611,7 +3641,7 @@
         <v>1827</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>28</v>
@@ -3637,7 +3667,7 @@
         <v>2141</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>28</v>
@@ -3663,7 +3693,7 @@
         <v>2141</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>28</v>
@@ -3689,7 +3719,7 @@
         <v>2141</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>28</v>
@@ -3715,7 +3745,7 @@
         <v>2141</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>28</v>
@@ -3741,7 +3771,7 @@
         <v>2141</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>28</v>
@@ -3767,7 +3797,7 @@
         <v>2141</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>28</v>
@@ -3793,7 +3823,7 @@
         <v>2141</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>28</v>
@@ -3819,7 +3849,7 @@
         <v>2141</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>28</v>
@@ -3845,7 +3875,7 @@
         <v>2141</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>28</v>
@@ -3871,7 +3901,7 @@
         <v>2141</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>28</v>
@@ -3897,7 +3927,7 @@
         <v>2141</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>28</v>
@@ -3923,7 +3953,7 @@
         <v>2141</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>28</v>
@@ -3949,7 +3979,7 @@
         <v>2395</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>28</v>
@@ -3975,7 +4005,7 @@
         <v>2395</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>28</v>
@@ -4001,7 +4031,7 @@
         <v>2395</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>28</v>
@@ -4027,7 +4057,7 @@
         <v>2395</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>28</v>
@@ -4053,7 +4083,7 @@
         <v>2395</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>28</v>
@@ -4079,7 +4109,7 @@
         <v>2395</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>28</v>
@@ -4105,7 +4135,7 @@
         <v>2395</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>28</v>
@@ -4131,7 +4161,7 @@
         <v>2395</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>28</v>
@@ -4157,7 +4187,7 @@
         <v>2395</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>28</v>
@@ -4183,7 +4213,7 @@
         <v>2395</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>28</v>
@@ -4209,7 +4239,7 @@
         <v>2656</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>28</v>
@@ -4235,7 +4265,7 @@
         <v>2656</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>28</v>
@@ -4261,7 +4291,7 @@
         <v>2656</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>28</v>
@@ -4287,7 +4317,7 @@
         <v>2656</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>28</v>
@@ -4313,7 +4343,7 @@
         <v>2656</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>28</v>
@@ -4339,7 +4369,7 @@
         <v>2656</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>28</v>
@@ -4365,7 +4395,7 @@
         <v>2656</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>28</v>
@@ -4391,7 +4421,7 @@
         <v>2656</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>28</v>
@@ -4417,7 +4447,7 @@
         <v>2656</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>28</v>
@@ -4443,7 +4473,7 @@
         <v>2656</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>28</v>
@@ -4469,7 +4499,7 @@
         <v>2656</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>28</v>
@@ -4495,7 +4525,7 @@
         <v>2656</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>28</v>
@@ -4521,7 +4551,7 @@
         <v>2915</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>28</v>
@@ -4547,7 +4577,7 @@
         <v>2915</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>28</v>
@@ -4573,7 +4603,7 @@
         <v>2915</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>28</v>
@@ -4599,7 +4629,7 @@
         <v>2915</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>28</v>
@@ -4625,7 +4655,7 @@
         <v>2915</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>28</v>
@@ -4651,7 +4681,7 @@
         <v>2915</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>28</v>
@@ -4677,7 +4707,7 @@
         <v>2915</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>28</v>
@@ -4703,7 +4733,7 @@
         <v>2915</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>28</v>
@@ -4729,7 +4759,7 @@
         <v>2915</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>28</v>
@@ -4755,7 +4785,7 @@
         <v>2915</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>28</v>
@@ -4781,7 +4811,7 @@
         <v>2915</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>28</v>
@@ -4807,7 +4837,7 @@
         <v>2915</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>28</v>
@@ -4833,7 +4863,7 @@
         <v>3181</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D130" s="6" t="s">
         <v>28</v>
@@ -4859,7 +4889,7 @@
         <v>3181</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>28</v>
@@ -4885,7 +4915,7 @@
         <v>3181</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D132" s="6" t="s">
         <v>28</v>
@@ -4911,7 +4941,7 @@
         <v>3181</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D133" s="6" t="s">
         <v>28</v>
@@ -4937,7 +4967,7 @@
         <v>3181</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D134" s="6" t="s">
         <v>28</v>
@@ -4963,7 +4993,7 @@
         <v>3181</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>28</v>
@@ -4989,7 +5019,7 @@
         <v>3181</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D136" s="6" t="s">
         <v>28</v>
@@ -5015,7 +5045,7 @@
         <v>3181</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D137" s="6" t="s">
         <v>28</v>
@@ -5041,7 +5071,7 @@
         <v>3181</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D138" s="6" t="s">
         <v>28</v>
@@ -5067,7 +5097,7 @@
         <v>3181</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D139" s="6" t="s">
         <v>28</v>
@@ -5093,7 +5123,7 @@
         <v>3388</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D140" s="6" t="s">
         <v>28</v>
@@ -5119,7 +5149,7 @@
         <v>3388</v>
       </c>
       <c r="C141" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D141" s="6" t="s">
         <v>28</v>
@@ -5145,7 +5175,7 @@
         <v>3388</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D142" s="6" t="s">
         <v>28</v>
@@ -5171,7 +5201,7 @@
         <v>3388</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D143" s="6" t="s">
         <v>28</v>
@@ -5197,7 +5227,7 @@
         <v>3388</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D144" s="6" t="s">
         <v>28</v>
@@ -5223,7 +5253,7 @@
         <v>3388</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D145" s="6" t="s">
         <v>28</v>
@@ -5249,7 +5279,7 @@
         <v>3388</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D146" s="6" t="s">
         <v>28</v>
@@ -5275,7 +5305,7 @@
         <v>3388</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D147" s="6" t="s">
         <v>28</v>
@@ -5301,7 +5331,7 @@
         <v>3388</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D148" s="6" t="s">
         <v>28</v>
@@ -5327,7 +5357,7 @@
         <v>3388</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>28</v>
@@ -5353,7 +5383,7 @@
         <v>3388</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D150" s="6" t="s">
         <v>28</v>
@@ -5379,7 +5409,7 @@
         <v>3673</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D151" s="6" t="s">
         <v>28</v>
@@ -5405,7 +5435,7 @@
         <v>3673</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D152" s="6" t="s">
         <v>28</v>
@@ -5431,7 +5461,7 @@
         <v>3673</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D153" s="6" t="s">
         <v>28</v>
@@ -5457,7 +5487,7 @@
         <v>3673</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D154" s="6" t="s">
         <v>28</v>
@@ -5483,7 +5513,7 @@
         <v>3673</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D155" s="6" t="s">
         <v>28</v>
@@ -5509,7 +5539,7 @@
         <v>3673</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D156" s="6" t="s">
         <v>28</v>
@@ -5535,7 +5565,7 @@
         <v>3673</v>
       </c>
       <c r="C157" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D157" s="6" t="s">
         <v>28</v>
@@ -5561,7 +5591,7 @@
         <v>3673</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D158" s="6" t="s">
         <v>28</v>
@@ -5587,7 +5617,7 @@
         <v>3673</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D159" s="6" t="s">
         <v>28</v>
@@ -5613,7 +5643,7 @@
         <v>3673</v>
       </c>
       <c r="C160" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D160" s="6" t="s">
         <v>28</v>
@@ -5639,7 +5669,7 @@
         <v>3673</v>
       </c>
       <c r="C161" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>28</v>
@@ -5665,7 +5695,7 @@
         <v>3673</v>
       </c>
       <c r="C162" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D162" s="6" t="s">
         <v>28</v>
@@ -5691,7 +5721,7 @@
         <v>3949</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D163" s="6" t="s">
         <v>28</v>
@@ -5717,7 +5747,7 @@
         <v>3949</v>
       </c>
       <c r="C164" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D164" s="6" t="s">
         <v>28</v>
@@ -5743,7 +5773,7 @@
         <v>3949</v>
       </c>
       <c r="C165" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D165" s="6" t="s">
         <v>28</v>
@@ -5769,7 +5799,7 @@
         <v>3949</v>
       </c>
       <c r="C166" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D166" s="6" t="s">
         <v>28</v>
@@ -5795,7 +5825,7 @@
         <v>3949</v>
       </c>
       <c r="C167" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D167" s="6" t="s">
         <v>28</v>
@@ -5821,7 +5851,7 @@
         <v>3949</v>
       </c>
       <c r="C168" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>28</v>
@@ -5847,7 +5877,7 @@
         <v>3949</v>
       </c>
       <c r="C169" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D169" s="6" t="s">
         <v>28</v>
@@ -5873,7 +5903,7 @@
         <v>3949</v>
       </c>
       <c r="C170" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D170" s="6" t="s">
         <v>28</v>
@@ -5899,7 +5929,7 @@
         <v>3949</v>
       </c>
       <c r="C171" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D171" s="6" t="s">
         <v>28</v>
@@ -5925,7 +5955,7 @@
         <v>3949</v>
       </c>
       <c r="C172" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D172" s="6" t="s">
         <v>28</v>
@@ -5951,7 +5981,7 @@
         <v>3949</v>
       </c>
       <c r="C173" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D173" s="6" t="s">
         <v>28</v>
@@ -5977,7 +6007,7 @@
         <v>3949</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D174" s="6" t="s">
         <v>28</v>
@@ -6003,7 +6033,7 @@
         <v>4267</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D175" s="6" t="s">
         <v>28</v>
@@ -6029,7 +6059,7 @@
         <v>4267</v>
       </c>
       <c r="C176" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D176" s="6" t="s">
         <v>28</v>
@@ -6055,7 +6085,7 @@
         <v>4267</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D177" s="6" t="s">
         <v>28</v>
@@ -6081,7 +6111,7 @@
         <v>4267</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D178" s="6" t="s">
         <v>28</v>
@@ -6107,7 +6137,7 @@
         <v>4267</v>
       </c>
       <c r="C179" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D179" s="6" t="s">
         <v>28</v>
@@ -6133,7 +6163,7 @@
         <v>4267</v>
       </c>
       <c r="C180" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D180" s="6" t="s">
         <v>28</v>
@@ -6159,7 +6189,7 @@
         <v>4267</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D181" s="6" t="s">
         <v>28</v>
@@ -6185,7 +6215,7 @@
         <v>4267</v>
       </c>
       <c r="C182" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D182" s="6" t="s">
         <v>28</v>
@@ -6211,7 +6241,7 @@
         <v>4267</v>
       </c>
       <c r="C183" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D183" s="6" t="s">
         <v>28</v>
@@ -6237,7 +6267,7 @@
         <v>4267</v>
       </c>
       <c r="C184" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D184" s="6" t="s">
         <v>28</v>
@@ -6263,7 +6293,7 @@
         <v>4267</v>
       </c>
       <c r="C185" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D185" s="6" t="s">
         <v>28</v>
@@ -6289,7 +6319,7 @@
         <v>4267</v>
       </c>
       <c r="C186" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D186" s="6" t="s">
         <v>28</v>
@@ -6315,7 +6345,7 @@
         <v>4473</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D187" s="6" t="s">
         <v>28</v>
@@ -6341,7 +6371,7 @@
         <v>4473</v>
       </c>
       <c r="C188" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D188" s="6" t="s">
         <v>28</v>
@@ -6367,7 +6397,7 @@
         <v>4473</v>
       </c>
       <c r="C189" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D189" s="6" t="s">
         <v>28</v>
@@ -6393,7 +6423,7 @@
         <v>4473</v>
       </c>
       <c r="C190" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D190" s="6" t="s">
         <v>28</v>
@@ -6419,7 +6449,7 @@
         <v>4473</v>
       </c>
       <c r="C191" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D191" s="6" t="s">
         <v>28</v>
@@ -6445,7 +6475,7 @@
         <v>4473</v>
       </c>
       <c r="C192" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D192" s="6" t="s">
         <v>28</v>
@@ -6471,7 +6501,7 @@
         <v>4473</v>
       </c>
       <c r="C193" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D193" s="6" t="s">
         <v>28</v>
@@ -6497,7 +6527,7 @@
         <v>4731</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D194" s="6" t="s">
         <v>28</v>
@@ -6523,7 +6553,7 @@
         <v>4731</v>
       </c>
       <c r="C195" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D195" s="6" t="s">
         <v>28</v>
@@ -6549,7 +6579,7 @@
         <v>4731</v>
       </c>
       <c r="C196" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D196" s="6" t="s">
         <v>28</v>
@@ -6575,7 +6605,7 @@
         <v>4731</v>
       </c>
       <c r="C197" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D197" s="6" t="s">
         <v>28</v>
@@ -6601,7 +6631,7 @@
         <v>4731</v>
       </c>
       <c r="C198" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D198" s="6" t="s">
         <v>28</v>
@@ -6627,7 +6657,7 @@
         <v>4731</v>
       </c>
       <c r="C199" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D199" s="6" t="s">
         <v>28</v>
@@ -6653,7 +6683,7 @@
         <v>4731</v>
       </c>
       <c r="C200" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D200" s="6" t="s">
         <v>28</v>
@@ -6679,7 +6709,7 @@
         <v>4731</v>
       </c>
       <c r="C201" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D201" s="6" t="s">
         <v>28</v>
@@ -6705,7 +6735,7 @@
         <v>4731</v>
       </c>
       <c r="C202" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D202" s="6" t="s">
         <v>28</v>
@@ -6731,7 +6761,7 @@
         <v>4731</v>
       </c>
       <c r="C203" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D203" s="6" t="s">
         <v>28</v>
@@ -6757,7 +6787,7 @@
         <v>4731</v>
       </c>
       <c r="C204" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D204" s="6" t="s">
         <v>28</v>
@@ -6783,7 +6813,7 @@
         <v>4972</v>
       </c>
       <c r="C205" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D205" s="6" t="s">
         <v>28</v>
@@ -6809,7 +6839,7 @@
         <v>4972</v>
       </c>
       <c r="C206" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D206" s="6" t="s">
         <v>28</v>
@@ -6835,7 +6865,7 @@
         <v>4972</v>
       </c>
       <c r="C207" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D207" s="6" t="s">
         <v>28</v>
@@ -6861,7 +6891,7 @@
         <v>4972</v>
       </c>
       <c r="C208" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D208" s="6" t="s">
         <v>28</v>
@@ -6887,7 +6917,7 @@
         <v>4972</v>
       </c>
       <c r="C209" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D209" s="6" t="s">
         <v>28</v>
@@ -6913,7 +6943,7 @@
         <v>4972</v>
       </c>
       <c r="C210" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D210" s="6" t="s">
         <v>28</v>
@@ -6939,7 +6969,7 @@
         <v>4972</v>
       </c>
       <c r="C211" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D211" s="6" t="s">
         <v>28</v>
@@ -6965,7 +6995,7 @@
         <v>4972</v>
       </c>
       <c r="C212" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D212" s="6" t="s">
         <v>28</v>
@@ -6991,7 +7021,7 @@
         <v>4972</v>
       </c>
       <c r="C213" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D213" s="6" t="s">
         <v>28</v>
@@ -7017,7 +7047,7 @@
         <v>4972</v>
       </c>
       <c r="C214" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D214" s="6" t="s">
         <v>28</v>
@@ -7043,7 +7073,7 @@
         <v>4972</v>
       </c>
       <c r="C215" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D215" s="6" t="s">
         <v>28</v>
@@ -7058,7 +7088,7 @@
         <v>6</v>
       </c>
       <c r="H215" s="11" t="s">
-        <v>239</v>
+        <v>323</v>
       </c>
     </row>
     <row r="216" spans="1:8" ht="16">
@@ -7069,7 +7099,7 @@
         <v>4972</v>
       </c>
       <c r="C216" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D216" s="6" t="s">
         <v>28</v>
@@ -7084,7 +7114,7 @@
         <v>6</v>
       </c>
       <c r="H216" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="217" spans="1:8" ht="16">
@@ -7095,7 +7125,7 @@
         <v>4972</v>
       </c>
       <c r="C217" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D217" s="6" t="s">
         <v>28</v>
@@ -7110,7 +7140,7 @@
         <v>6</v>
       </c>
       <c r="H217" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="218" spans="1:8" ht="16">
@@ -7121,7 +7151,7 @@
         <v>4972</v>
       </c>
       <c r="C218" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D218" s="6" t="s">
         <v>28</v>
@@ -7136,7 +7166,7 @@
         <v>6</v>
       </c>
       <c r="H218" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="219" spans="1:8" ht="16">
@@ -7147,7 +7177,7 @@
         <v>5296</v>
       </c>
       <c r="C219" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D219" s="6" t="s">
         <v>28</v>
@@ -7156,13 +7186,13 @@
         <v>9</v>
       </c>
       <c r="F219" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G219" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H219" s="10" t="s">
-        <v>229</v>
+        <v>313</v>
       </c>
     </row>
     <row r="220" spans="1:8" ht="16">
@@ -7173,7 +7203,7 @@
         <v>5296</v>
       </c>
       <c r="C220" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D220" s="6" t="s">
         <v>28</v>
@@ -7182,13 +7212,13 @@
         <v>9</v>
       </c>
       <c r="F220" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G220" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H220" s="10" t="s">
-        <v>230</v>
+        <v>314</v>
       </c>
     </row>
     <row r="221" spans="1:8" ht="16">
@@ -7199,7 +7229,7 @@
         <v>5296</v>
       </c>
       <c r="C221" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D221" s="6" t="s">
         <v>28</v>
@@ -7208,13 +7238,13 @@
         <v>9</v>
       </c>
       <c r="F221" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G221" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H221" s="10" t="s">
-        <v>231</v>
+        <v>315</v>
       </c>
     </row>
     <row r="222" spans="1:8" ht="16">
@@ -7225,7 +7255,7 @@
         <v>5296</v>
       </c>
       <c r="C222" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D222" s="6" t="s">
         <v>28</v>
@@ -7234,13 +7264,13 @@
         <v>9</v>
       </c>
       <c r="F222" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G222" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H222" s="10" t="s">
-        <v>232</v>
+        <v>316</v>
       </c>
     </row>
     <row r="223" spans="1:8" ht="16">
@@ -7251,7 +7281,7 @@
         <v>5296</v>
       </c>
       <c r="C223" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D223" s="6" t="s">
         <v>28</v>
@@ -7260,13 +7290,13 @@
         <v>9</v>
       </c>
       <c r="F223" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G223" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H223" s="10" t="s">
-        <v>233</v>
+        <v>317</v>
       </c>
     </row>
     <row r="224" spans="1:8" ht="16">
@@ -7277,7 +7307,7 @@
         <v>5296</v>
       </c>
       <c r="C224" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D224" s="6" t="s">
         <v>28</v>
@@ -7286,13 +7316,13 @@
         <v>8</v>
       </c>
       <c r="F224" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G224" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H224" s="10" t="s">
-        <v>234</v>
+        <v>318</v>
       </c>
     </row>
     <row r="225" spans="1:8" ht="16">
@@ -7303,7 +7333,7 @@
         <v>5296</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D225" s="6" t="s">
         <v>28</v>
@@ -7312,13 +7342,13 @@
         <v>8</v>
       </c>
       <c r="F225" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G225" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H225" s="10" t="s">
-        <v>235</v>
+        <v>319</v>
       </c>
     </row>
     <row r="226" spans="1:8" ht="13">
@@ -7329,7 +7359,7 @@
         <v>5296</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D226" s="6" t="s">
         <v>28</v>
@@ -7338,13 +7368,13 @@
         <v>11</v>
       </c>
       <c r="F226" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G226" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H226" s="11" t="s">
-        <v>239</v>
+        <v>320</v>
       </c>
     </row>
     <row r="227" spans="1:8" ht="16">
@@ -7355,7 +7385,7 @@
         <v>5296</v>
       </c>
       <c r="C227" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D227" s="6" t="s">
         <v>28</v>
@@ -7364,13 +7394,13 @@
         <v>41</v>
       </c>
       <c r="F227" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G227" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H227" s="14" t="s">
-        <v>242</v>
+        <v>321</v>
       </c>
     </row>
     <row r="228" spans="1:8" ht="16">
@@ -7381,7 +7411,7 @@
         <v>5546</v>
       </c>
       <c r="C228" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D228" s="15" t="s">
         <v>28</v>
@@ -7390,13 +7420,13 @@
         <v>9</v>
       </c>
       <c r="F228" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="G228" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H228" s="18" t="s">
         <v>244</v>
-      </c>
-      <c r="G228" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H228" s="18" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="229" spans="1:8" ht="16">
@@ -7407,7 +7437,7 @@
         <v>5546</v>
       </c>
       <c r="C229" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D229" s="16" t="s">
         <v>28</v>
@@ -7416,13 +7446,13 @@
         <v>9</v>
       </c>
       <c r="F229" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G229" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H229" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="230" spans="1:8" ht="16">
@@ -7433,7 +7463,7 @@
         <v>5546</v>
       </c>
       <c r="C230" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D230" s="16" t="s">
         <v>28</v>
@@ -7442,13 +7472,13 @@
         <v>9</v>
       </c>
       <c r="F230" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G230" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H230" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="231" spans="1:8" ht="16">
@@ -7459,7 +7489,7 @@
         <v>5546</v>
       </c>
       <c r="C231" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D231" s="16" t="s">
         <v>28</v>
@@ -7468,13 +7498,13 @@
         <v>9</v>
       </c>
       <c r="F231" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G231" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H231" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="232" spans="1:8" ht="16">
@@ -7485,7 +7515,7 @@
         <v>5546</v>
       </c>
       <c r="C232" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D232" s="16" t="s">
         <v>28</v>
@@ -7494,13 +7524,13 @@
         <v>9</v>
       </c>
       <c r="F232" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G232" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H232" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="233" spans="1:8" ht="16">
@@ -7511,7 +7541,7 @@
         <v>5546</v>
       </c>
       <c r="C233" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D233" s="16" t="s">
         <v>28</v>
@@ -7520,13 +7550,13 @@
         <v>8</v>
       </c>
       <c r="F233" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G233" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H233" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="234" spans="1:8" ht="16">
@@ -7537,7 +7567,7 @@
         <v>5546</v>
       </c>
       <c r="C234" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D234" s="16" t="s">
         <v>28</v>
@@ -7546,13 +7576,13 @@
         <v>8</v>
       </c>
       <c r="F234" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G234" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H234" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="235" spans="1:8" ht="16">
@@ -7563,7 +7593,7 @@
         <v>5546</v>
       </c>
       <c r="C235" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D235" s="16" t="s">
         <v>28</v>
@@ -7572,13 +7602,13 @@
         <v>8</v>
       </c>
       <c r="F235" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G235" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H235" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="236" spans="1:8" ht="13">
@@ -7589,7 +7619,7 @@
         <v>5546</v>
       </c>
       <c r="C236" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D236" s="16" t="s">
         <v>28</v>
@@ -7598,13 +7628,13 @@
         <v>11</v>
       </c>
       <c r="F236" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G236" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H236" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="237" spans="1:8" ht="16">
@@ -7615,7 +7645,7 @@
         <v>5546</v>
       </c>
       <c r="C237" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D237" s="16" t="s">
         <v>28</v>
@@ -7624,13 +7654,13 @@
         <v>41</v>
       </c>
       <c r="F237" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G237" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H237" s="14" t="s">
-        <v>160</v>
+        <v>322</v>
       </c>
     </row>
     <row r="238" spans="1:8" ht="16">
@@ -7641,7 +7671,7 @@
         <v>5803</v>
       </c>
       <c r="C238" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D238" s="16" t="s">
         <v>28</v>
@@ -7650,13 +7680,13 @@
         <v>9</v>
       </c>
       <c r="F238" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="G238" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H238" s="18" t="s">
         <v>254</v>
-      </c>
-      <c r="G238" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H238" s="18" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="239" spans="1:8" ht="16">
@@ -7667,7 +7697,7 @@
         <v>5803</v>
       </c>
       <c r="C239" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D239" s="16" t="s">
         <v>28</v>
@@ -7676,13 +7706,13 @@
         <v>9</v>
       </c>
       <c r="F239" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G239" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H239" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="240" spans="1:8" ht="16">
@@ -7693,7 +7723,7 @@
         <v>5803</v>
       </c>
       <c r="C240" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D240" s="16" t="s">
         <v>28</v>
@@ -7702,13 +7732,13 @@
         <v>9</v>
       </c>
       <c r="F240" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G240" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H240" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="241" spans="1:8" ht="16">
@@ -7719,7 +7749,7 @@
         <v>5803</v>
       </c>
       <c r="C241" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D241" s="16" t="s">
         <v>28</v>
@@ -7728,13 +7758,13 @@
         <v>9</v>
       </c>
       <c r="F241" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G241" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H241" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="242" spans="1:8" ht="16">
@@ -7745,7 +7775,7 @@
         <v>5803</v>
       </c>
       <c r="C242" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D242" s="16" t="s">
         <v>28</v>
@@ -7754,13 +7784,13 @@
         <v>9</v>
       </c>
       <c r="F242" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G242" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H242" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="243" spans="1:8" ht="16">
@@ -7771,7 +7801,7 @@
         <v>5803</v>
       </c>
       <c r="C243" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D243" s="16" t="s">
         <v>28</v>
@@ -7780,13 +7810,13 @@
         <v>8</v>
       </c>
       <c r="F243" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G243" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H243" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="244" spans="1:8" ht="16">
@@ -7797,7 +7827,7 @@
         <v>5803</v>
       </c>
       <c r="C244" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D244" s="16" t="s">
         <v>28</v>
@@ -7806,13 +7836,13 @@
         <v>8</v>
       </c>
       <c r="F244" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G244" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H244" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="245" spans="1:8" ht="16">
@@ -7823,7 +7853,7 @@
         <v>5803</v>
       </c>
       <c r="C245" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D245" s="16" t="s">
         <v>28</v>
@@ -7832,13 +7862,13 @@
         <v>8</v>
       </c>
       <c r="F245" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G245" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H245" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="246" spans="1:8" ht="13">
@@ -7849,7 +7879,7 @@
         <v>5803</v>
       </c>
       <c r="C246" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D246" s="16" t="s">
         <v>28</v>
@@ -7858,13 +7888,13 @@
         <v>8</v>
       </c>
       <c r="F246" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G246" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H246" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="247" spans="1:8" ht="13">
@@ -7875,7 +7905,7 @@
         <v>5803</v>
       </c>
       <c r="C247" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D247" s="16" t="s">
         <v>28</v>
@@ -7884,13 +7914,13 @@
         <v>11</v>
       </c>
       <c r="F247" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G247" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H247" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="248" spans="1:8" ht="16">
@@ -7901,7 +7931,7 @@
         <v>5803</v>
       </c>
       <c r="C248" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D248" s="16" t="s">
         <v>28</v>
@@ -7910,13 +7940,13 @@
         <v>41</v>
       </c>
       <c r="F248" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G248" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H248" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="249" spans="1:8" ht="16">
@@ -7927,7 +7957,7 @@
         <v>6104</v>
       </c>
       <c r="C249" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D249" s="6" t="s">
         <v>28</v>
@@ -7936,13 +7966,13 @@
         <v>9</v>
       </c>
       <c r="F249" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G249" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H249" s="10" t="s">
         <v>266</v>
-      </c>
-      <c r="G249" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H249" s="10" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="250" spans="1:8" ht="16">
@@ -7953,7 +7983,7 @@
         <v>6104</v>
       </c>
       <c r="C250" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D250" s="6" t="s">
         <v>28</v>
@@ -7962,13 +7992,13 @@
         <v>9</v>
       </c>
       <c r="F250" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G250" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H250" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="251" spans="1:8" ht="16">
@@ -7979,7 +8009,7 @@
         <v>6104</v>
       </c>
       <c r="C251" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D251" s="6" t="s">
         <v>28</v>
@@ -7988,13 +8018,13 @@
         <v>9</v>
       </c>
       <c r="F251" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G251" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H251" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="252" spans="1:8" ht="16">
@@ -8005,7 +8035,7 @@
         <v>6104</v>
       </c>
       <c r="C252" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D252" s="6" t="s">
         <v>28</v>
@@ -8014,13 +8044,13 @@
         <v>9</v>
       </c>
       <c r="F252" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G252" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H252" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="253" spans="1:8" ht="16">
@@ -8031,7 +8061,7 @@
         <v>6104</v>
       </c>
       <c r="C253" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D253" s="6" t="s">
         <v>28</v>
@@ -8040,13 +8070,13 @@
         <v>9</v>
       </c>
       <c r="F253" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G253" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H253" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="254" spans="1:8" ht="16">
@@ -8057,7 +8087,7 @@
         <v>6104</v>
       </c>
       <c r="C254" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D254" s="6" t="s">
         <v>28</v>
@@ -8066,13 +8096,13 @@
         <v>8</v>
       </c>
       <c r="F254" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G254" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H254" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="255" spans="1:8" ht="16">
@@ -8083,7 +8113,7 @@
         <v>6104</v>
       </c>
       <c r="C255" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D255" s="6" t="s">
         <v>28</v>
@@ -8092,13 +8122,13 @@
         <v>8</v>
       </c>
       <c r="F255" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G255" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H255" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="256" spans="1:8" ht="16">
@@ -8109,7 +8139,7 @@
         <v>6104</v>
       </c>
       <c r="C256" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D256" s="6" t="s">
         <v>28</v>
@@ -8118,13 +8148,13 @@
         <v>8</v>
       </c>
       <c r="F256" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G256" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H256" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="257" spans="1:11" ht="16">
@@ -8135,7 +8165,7 @@
         <v>6104</v>
       </c>
       <c r="C257" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D257" s="6" t="s">
         <v>28</v>
@@ -8144,13 +8174,13 @@
         <v>8</v>
       </c>
       <c r="F257" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G257" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H257" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="258" spans="1:11" ht="13">
@@ -8161,7 +8191,7 @@
         <v>6104</v>
       </c>
       <c r="C258" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D258" s="6" t="s">
         <v>28</v>
@@ -8170,13 +8200,13 @@
         <v>11</v>
       </c>
       <c r="F258" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G258" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H258" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="259" spans="1:11" ht="16">
@@ -8187,7 +8217,7 @@
         <v>6104</v>
       </c>
       <c r="C259" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D259" s="6" t="s">
         <v>28</v>
@@ -8196,13 +8226,13 @@
         <v>41</v>
       </c>
       <c r="F259" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G259" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H259" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="260" spans="1:11" ht="16">
@@ -8213,7 +8243,7 @@
         <v>6322</v>
       </c>
       <c r="C260" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D260" s="6" t="s">
         <v>28</v>
@@ -8222,13 +8252,13 @@
         <v>9</v>
       </c>
       <c r="F260" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="G260" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H260" s="10" t="s">
         <v>278</v>
-      </c>
-      <c r="G260" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H260" s="10" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="261" spans="1:11" ht="16">
@@ -8239,7 +8269,7 @@
         <v>6322</v>
       </c>
       <c r="C261" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D261" s="6" t="s">
         <v>28</v>
@@ -8248,13 +8278,13 @@
         <v>9</v>
       </c>
       <c r="F261" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G261" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H261" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K261" s="25"/>
     </row>
@@ -8266,7 +8296,7 @@
         <v>6322</v>
       </c>
       <c r="C262" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D262" s="6" t="s">
         <v>28</v>
@@ -8275,13 +8305,13 @@
         <v>9</v>
       </c>
       <c r="F262" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G262" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H262" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K262" s="25"/>
     </row>
@@ -8293,7 +8323,7 @@
         <v>6322</v>
       </c>
       <c r="C263" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D263" s="6" t="s">
         <v>28</v>
@@ -8302,13 +8332,13 @@
         <v>9</v>
       </c>
       <c r="F263" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G263" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H263" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K263" s="25"/>
     </row>
@@ -8320,7 +8350,7 @@
         <v>6322</v>
       </c>
       <c r="C264" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D264" s="6" t="s">
         <v>28</v>
@@ -8329,13 +8359,13 @@
         <v>9</v>
       </c>
       <c r="F264" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G264" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H264" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K264" s="25"/>
     </row>
@@ -8347,7 +8377,7 @@
         <v>6322</v>
       </c>
       <c r="C265" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D265" s="6" t="s">
         <v>28</v>
@@ -8356,13 +8386,13 @@
         <v>8</v>
       </c>
       <c r="F265" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G265" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H265" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K265" s="25"/>
     </row>
@@ -8374,7 +8404,7 @@
         <v>6322</v>
       </c>
       <c r="C266" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D266" s="6" t="s">
         <v>28</v>
@@ -8383,13 +8413,13 @@
         <v>11</v>
       </c>
       <c r="F266" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G266" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H266" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K266" s="25"/>
     </row>
@@ -8401,7 +8431,7 @@
         <v>6322</v>
       </c>
       <c r="C267" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D267" s="6" t="s">
         <v>28</v>
@@ -8410,13 +8440,13 @@
         <v>41</v>
       </c>
       <c r="F267" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G267" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H267" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K267" s="25"/>
     </row>
@@ -8428,7 +8458,7 @@
         <v>6322</v>
       </c>
       <c r="C268" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D268" s="6" t="s">
         <v>28</v>
@@ -8437,13 +8467,13 @@
         <v>9</v>
       </c>
       <c r="F268" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="G268" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H268" s="10" t="s">
         <v>287</v>
-      </c>
-      <c r="G268" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H268" s="10" t="s">
-        <v>288</v>
       </c>
       <c r="K268" s="25"/>
     </row>
@@ -8455,7 +8485,7 @@
         <v>6322</v>
       </c>
       <c r="C269" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D269" s="6" t="s">
         <v>28</v>
@@ -8464,13 +8494,13 @@
         <v>9</v>
       </c>
       <c r="F269" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G269" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H269" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K269" s="25"/>
     </row>
@@ -8482,7 +8512,7 @@
         <v>6322</v>
       </c>
       <c r="C270" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D270" s="6" t="s">
         <v>28</v>
@@ -8491,13 +8521,13 @@
         <v>9</v>
       </c>
       <c r="F270" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G270" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H270" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K270" s="25"/>
     </row>
@@ -8509,7 +8539,7 @@
         <v>6322</v>
       </c>
       <c r="C271" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D271" s="6" t="s">
         <v>28</v>
@@ -8518,13 +8548,13 @@
         <v>9</v>
       </c>
       <c r="F271" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G271" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H271" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K271" s="25"/>
     </row>
@@ -8536,7 +8566,7 @@
         <v>6322</v>
       </c>
       <c r="C272" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D272" s="6" t="s">
         <v>28</v>
@@ -8545,13 +8575,13 @@
         <v>9</v>
       </c>
       <c r="F272" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G272" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H272" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K272" s="25"/>
     </row>
@@ -8563,7 +8593,7 @@
         <v>6322</v>
       </c>
       <c r="C273" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D273" s="6" t="s">
         <v>28</v>
@@ -8572,13 +8602,13 @@
         <v>41</v>
       </c>
       <c r="F273" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G273" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H273" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K273" s="25"/>
     </row>
@@ -8623,7 +8653,7 @@
         <v>4</v>
       </c>
       <c r="E275" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F275" s="7" t="s">
         <v>4</v>
@@ -8632,7 +8662,7 @@
         <v>6</v>
       </c>
       <c r="H275" s="21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K275" s="25"/>
     </row>

</xml_diff>